<commit_message>
Upd: 调整 Excel 数据
- 处理导入数据的脚本，像病害那样对前面的层级进行顿号分隔处理
- 重新录入基础数据和路径数据
- 调整基础权重的 Excel 数据
- 重新导入权重基础数据
</commit_message>
<xml_diff>
--- a/static/weight_base.xlsx
+++ b/static/weight_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/GitHub/PresentationLayer/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A316B287-522A-314D-81E9-B19BADA73549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF266397-006A-034F-A664-7FADF9436960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1260" windowWidth="27700" windowHeight="16700" xr2:uid="{40E09B35-1B98-D544-942B-D63CFA7FB7D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="66">
   <si>
     <t>桥梁类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,24 +57,12 @@
     <t>上部结构</t>
   </si>
   <si>
-    <t>上部承重构件（主梁、挂梁）</t>
-  </si>
-  <si>
-    <t>上部一般构件（湿接缝、横隔板等）</t>
-  </si>
-  <si>
     <t>支座</t>
   </si>
   <si>
     <t>下部结构</t>
   </si>
   <si>
-    <t>翼墙、耳墙</t>
-  </si>
-  <si>
-    <t>锥坡、护坡</t>
-  </si>
-  <si>
     <t>桥墩</t>
   </si>
   <si>
@@ -100,15 +88,6 @@
   </si>
   <si>
     <t>人行道</t>
-  </si>
-  <si>
-    <t>栏杆、护栏</t>
-  </si>
-  <si>
-    <t>排水系统</t>
-  </si>
-  <si>
-    <t>照明、标志</t>
   </si>
   <si>
     <t>梁式桥</t>
@@ -141,21 +120,11 @@
     <t>钢梁桥</t>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>钢筋混凝土拱桥（板拱桥、肋拱桥和箱拱桥）</t>
-  </si>
-  <si>
     <t>钢筋混凝土拱桥
 （双曲拱桥）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>刚架拱片（桁架拱片）</t>
-  </si>
-  <si>
     <t>横向联结系</t>
   </si>
   <si>
@@ -178,9 +147,6 @@
     <t>吊杆</t>
   </si>
   <si>
-    <t>系杆(含锚具)</t>
-  </si>
-  <si>
     <t>桥面板（梁）</t>
   </si>
   <si>
@@ -211,19 +177,95 @@
     <t>锚促</t>
   </si>
   <si>
+    <t>散索鞍</t>
+  </si>
+  <si>
+    <t>主梁</t>
+  </si>
+  <si>
+    <t>斜拉桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下部结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桥面系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上部承重构件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上部一般构件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护栏</t>
+  </si>
+  <si>
+    <t>标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栏杆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耳墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>翼墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锥坡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>护坡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>索塔基础</t>
-  </si>
-  <si>
-    <t>散索鞍</t>
-  </si>
-  <si>
-    <t>斜拉索系统（斜拉索、锚具、拉索护套、减震装置等）</t>
-  </si>
-  <si>
-    <t>主梁</t>
-  </si>
-  <si>
-    <t>斜拉桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防排水系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢筋混凝土拱桥（板拱桥、肋拱桥和箱拱桥）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桁架拱片</t>
+  </si>
+  <si>
+    <t>桁架拱片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刚架拱片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系杆及防护板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斜拉索系统</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -641,16 +683,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5D4DB8-0539-6849-B6BB-CF42055FAE5A}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" customWidth="1"/>
+    <col min="4" max="4" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
@@ -661,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -672,16 +715,16 @@
     </row>
     <row r="2" spans="1:5" ht="97" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1">
         <v>0.7</v>
@@ -691,10 +734,10 @@
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1">
         <v>0.18</v>
@@ -704,10 +747,10 @@
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1">
         <v>0.12</v>
@@ -716,13 +759,13 @@
     <row r="5" spans="1:5" ht="18">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
         <v>0.02</v>
@@ -733,10 +776,10 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18">
@@ -744,10 +787,10 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18">
@@ -755,10 +798,10 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18">
@@ -766,10 +809,10 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18">
@@ -777,10 +820,10 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18">
@@ -788,25 +831,21 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
-        <v>0.02</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18">
       <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1">
-        <v>0.4</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18">
@@ -814,21 +853,25 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1">
-        <v>0.25</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18">
@@ -836,10 +879,10 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18">
@@ -847,7 +890,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
         <v>0.1</v>
@@ -858,108 +901,106 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18">
-      <c r="A18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="1" t="s">
-        <v>26</v>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E19" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E20" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="38" customHeight="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1">
         <v>0.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E23" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="38" customHeight="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="C24" s="6"/>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="38" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E25" s="1">
-        <v>0.25</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18">
@@ -967,123 +1008,125 @@
       <c r="B26" s="5"/>
       <c r="C26" s="7"/>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E26" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="38" customHeight="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="7" t="s">
-        <v>38</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E28" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="38" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="7"/>
       <c r="D29" s="1" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="E29" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18">
       <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E30" s="1">
-        <v>0.02</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
+      <c r="C32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E32" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="38" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="1" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="E33" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E34" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E36" s="1">
         <v>0.02</v>
@@ -1091,17 +1134,13 @@
     </row>
     <row r="37" spans="1:5" ht="18">
       <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E37" s="1">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18">
@@ -1109,10 +1148,10 @@
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E38" s="1">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18">
@@ -1120,10 +1159,10 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E39" s="1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18">
@@ -1131,10 +1170,10 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18">
@@ -1142,10 +1181,10 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E41" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18">
@@ -1153,383 +1192,377 @@
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E42" s="1">
-        <v>0.05</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18">
-      <c r="A43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1">
-        <v>0.28000000000000003</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E44" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18">
       <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="4"/>
+      <c r="B45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E45" s="1">
-        <v>0.13</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="4"/>
+      <c r="C46" s="5"/>
       <c r="D46" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E46" s="1">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="4"/>
+      <c r="C47" s="5"/>
       <c r="D47" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="E47" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="4"/>
+      <c r="C48" s="5"/>
       <c r="D48" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E48" s="1">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18">
       <c r="A49" s="4"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="4"/>
+      <c r="C49" s="5"/>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E49" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18">
       <c r="A50" s="4"/>
-      <c r="B50" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>9</v>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E50" s="1">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="4"/>
+      <c r="C51" s="5"/>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E51" s="1">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18">
       <c r="A52" s="4"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="4"/>
+      <c r="C52" s="5"/>
       <c r="D52" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E52" s="1">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18">
-      <c r="A53" s="4"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D53" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E53" s="1">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18">
       <c r="A54" s="4"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="4"/>
+      <c r="C54" s="5"/>
       <c r="D54" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E54" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="4"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E55" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18">
       <c r="A56" s="4"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="4"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E56" s="1">
-        <v>0.02</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18">
       <c r="A57" s="4"/>
-      <c r="B57" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
       <c r="D57" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="E57" s="1">
-        <v>0.4</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18">
       <c r="A58" s="4"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="4"/>
+      <c r="C58" s="5"/>
       <c r="D58" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E58" s="1">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18">
       <c r="A59" s="4"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="4"/>
+      <c r="C59" s="5"/>
       <c r="D59" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18">
       <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="4"/>
+      <c r="B60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D60" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E60" s="1">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="4"/>
+      <c r="C61" s="5"/>
       <c r="D61" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="E61" s="1">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18">
       <c r="A62" s="4"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="4"/>
+      <c r="C62" s="5"/>
       <c r="D62" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E62" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18">
-      <c r="A63" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
       <c r="D63" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E63" s="1">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18">
       <c r="A64" s="4"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="4"/>
+      <c r="C64" s="5"/>
       <c r="D64" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="4"/>
+      <c r="C65" s="5"/>
       <c r="D65" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18">
       <c r="A66" s="4"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="4"/>
+      <c r="C66" s="5"/>
       <c r="D66" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E66" s="1">
-        <v>0.04</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18">
       <c r="A67" s="4"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="4"/>
+      <c r="C67" s="5"/>
       <c r="D67" s="1" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E67" s="1">
-        <v>0.25</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="4"/>
+      <c r="C68" s="5"/>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E68" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18">
       <c r="A69" s="4"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="4"/>
+      <c r="B69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E69" s="1">
-        <v>0.17</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18">
       <c r="A70" s="4"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="4"/>
+      <c r="C70" s="5"/>
       <c r="D70" s="1" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="E70" s="1">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="4"/>
+      <c r="C71" s="5"/>
       <c r="D71" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E71" s="1">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18">
       <c r="A72" s="4"/>
-      <c r="B72" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
       <c r="D72" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E72" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18">
       <c r="A73" s="4"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="4"/>
+      <c r="C73" s="5"/>
       <c r="D73" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E73" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="1" t="s">
-        <v>14</v>
+      <c r="C74" s="5"/>
+      <c r="D74" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E74" s="1">
         <v>0.1</v>
@@ -1538,9 +1571,9 @@
     <row r="75" spans="1:5" ht="18">
       <c r="A75" s="4"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="4"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="E75" s="1">
         <v>0.05</v>
@@ -1548,237 +1581,233 @@
     </row>
     <row r="76" spans="1:5" ht="18">
       <c r="A76" s="4"/>
-      <c r="B76" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
       <c r="D76" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="E76" s="1">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18">
-      <c r="A77" s="4"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="4"/>
+      <c r="A77" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D77" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E77" s="1">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
-      <c r="C78" s="4"/>
+      <c r="C78" s="5"/>
       <c r="D78" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E78" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="4"/>
+      <c r="C79" s="5"/>
       <c r="D79" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E79" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
-      <c r="C80" s="4"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E80" s="1">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18">
       <c r="A81" s="4"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="4"/>
+      <c r="C81" s="5"/>
       <c r="D81" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E81" s="1">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18">
-      <c r="A82" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
       <c r="D82" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E82" s="1">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="4"/>
+      <c r="C83" s="5"/>
       <c r="D83" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E83" s="1">
-        <v>0.25</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
-      <c r="C84" s="4"/>
+      <c r="C84" s="5"/>
       <c r="D84" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E84" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18">
       <c r="A85" s="4"/>
       <c r="B85" s="5"/>
-      <c r="C85" s="4"/>
+      <c r="C85" s="5"/>
       <c r="D85" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="E85" s="1">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18">
       <c r="A86" s="4"/>
       <c r="B86" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E86" s="1">
-        <v>0.02</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
-      <c r="C87" s="4"/>
+      <c r="C87" s="5"/>
       <c r="D87" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E87" s="1">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
-      <c r="C88" s="4"/>
+      <c r="C88" s="5"/>
       <c r="D88" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E88" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
-      <c r="C89" s="4"/>
+      <c r="C89" s="5"/>
       <c r="D89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E89" s="1">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18">
       <c r="A90" s="4"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="4"/>
+      <c r="B90" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E90" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
-      <c r="C91" s="4"/>
+      <c r="C91" s="5"/>
       <c r="D91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E91" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
-      <c r="C92" s="4"/>
+      <c r="C92" s="5"/>
       <c r="D92" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E92" s="1">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18">
       <c r="A93" s="4"/>
-      <c r="B93" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
       <c r="D93" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E93" s="1">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18">
       <c r="A94" s="4"/>
       <c r="B94" s="5"/>
-      <c r="C94" s="4"/>
+      <c r="C94" s="5"/>
       <c r="D94" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="E94" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="1" t="s">
-        <v>19</v>
+      <c r="C95" s="5"/>
+      <c r="D95" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E95" s="1">
         <v>0.1</v>
@@ -1787,75 +1816,309 @@
     <row r="96" spans="1:5" ht="18">
       <c r="A96" s="4"/>
       <c r="B96" s="5"/>
-      <c r="C96" s="4"/>
+      <c r="C96" s="5"/>
       <c r="D96" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E96" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="18">
       <c r="A97" s="4"/>
       <c r="B97" s="5"/>
-      <c r="C97" s="4"/>
+      <c r="C97" s="5"/>
       <c r="D97" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E97" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="18">
-      <c r="A98" s="4"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="4"/>
+      <c r="A98" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D98" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E98" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="18">
+      <c r="A99" s="4"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="18">
+      <c r="A100" s="4"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="18">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="18">
+      <c r="A102" s="4"/>
+      <c r="B102" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="18">
+      <c r="A103" s="4"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="18">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="18">
+      <c r="A105" s="4"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="18">
+      <c r="A106" s="4"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="18">
+      <c r="A107" s="4"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="18">
+      <c r="A108" s="4"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="18">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E109" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="18">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="18">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="18">
+      <c r="A112" s="4"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="18">
+      <c r="A113" s="4"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="18">
+      <c r="A114" s="4"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="18">
+      <c r="A115" s="4"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="18">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="18">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="18">
+      <c r="A118" s="4"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="1">
         <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A82:A98"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B93:B98"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="C86:C92"/>
-    <mergeCell ref="C93:C98"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="B57:B62"/>
-    <mergeCell ref="A43:A62"/>
-    <mergeCell ref="A63:A81"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B81"/>
-    <mergeCell ref="C63:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C76:C81"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C30:C36"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="C43:C49"/>
-    <mergeCell ref="C50:C56"/>
-    <mergeCell ref="A18:A42"/>
-    <mergeCell ref="B18:B29"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A2:A21"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="C5:C11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="C5:C13"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="C14:C21"/>
+    <mergeCell ref="A22:A52"/>
+    <mergeCell ref="B22:B35"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="B36:B44"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B45:B52"/>
+    <mergeCell ref="C36:C44"/>
+    <mergeCell ref="C45:C52"/>
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="B60:B68"/>
+    <mergeCell ref="C53:C59"/>
+    <mergeCell ref="C60:C68"/>
+    <mergeCell ref="C69:C76"/>
+    <mergeCell ref="B69:B76"/>
+    <mergeCell ref="A53:A76"/>
+    <mergeCell ref="A77:A97"/>
+    <mergeCell ref="B77:B85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B90:B97"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="C86:C89"/>
+    <mergeCell ref="C90:C97"/>
+    <mergeCell ref="A98:A118"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="B102:B110"/>
+    <mergeCell ref="B111:B118"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="C102:C110"/>
+    <mergeCell ref="C111:C118"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>